<commit_message>
fixed some issues form customer import
</commit_message>
<xml_diff>
--- a/public/import_template/customer_import_template.xlsx
+++ b/public/import_template/customer_import_template.xlsx
@@ -98,7 +98,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -157,8 +157,8 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -466,7 +466,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +494,7 @@
     <col min="11" max="11" width="22.85546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="1"/>
     <col min="14" max="14" width="16.28515625" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="1" customWidth="1"/>
     <col min="16" max="16" width="26.7109375" customWidth="1"/>
     <col min="17" max="17" width="16.42578125" style="6" customWidth="1"/>
     <col min="18" max="18" width="25.140625" style="6" customWidth="1"/>
@@ -541,10 +541,10 @@
         <v>6</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>9</v>

</xml_diff>